<commit_message>
Modifica istanza CIB (su segnalazione ETL un segment era associato al WS errato)
</commit_message>
<xml_diff>
--- a/earlywarning-pom/earlywarning-config/src/baf-instances/45_Inst_Workspace_CIB.xlsx
+++ b/earlywarning-pom/earlywarning-config/src/baf-instances/45_Inst_Workspace_CIB.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="465" windowWidth="28215" windowHeight="15135"/>
+    <workbookView xWindow="2040" yWindow="465" windowWidth="28215" windowHeight="15135" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Workspace" sheetId="1" r:id="rId1"/>
@@ -1044,7 +1044,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
@@ -1223,8 +1223,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1328,7 +1328,7 @@
         <v>43</v>
       </c>
       <c r="E6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F6" t="s">
         <v>44</v>

</xml_diff>